<commit_message>
Added new user stories.
</commit_message>
<xml_diff>
--- a/UserStories/arslan/User_Stories.xlsx
+++ b/UserStories/arslan/User_Stories.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t xml:space="preserve"> Βήματα διεργασίας SCRUM</t>
   </si>
@@ -141,45 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ως &lt;τύπος χρήστη&gt;, θέλω να &lt;κάνω … &gt; ώστε να &lt;επωφεληθώ ...&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ως μη-ταυτοποιημένος χρήστης θέλω να  </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-      </rPr>
-      <t xml:space="preserve">δημιουργήσω λογαριασμό </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-      </rPr>
-      <t xml:space="preserve">για να έχω πρόσβαση στο σύστημα</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Στο UI εισάγω τα στοιχεία μου (ονοματεπώνυμο, κλπ, email, username, passw) και δημιουργείται ο λογαριασμός μου</t>
   </si>
   <si>
     <t xml:space="preserve">US02</t>
@@ -246,7 +207,7 @@
     <t xml:space="preserve">Ως καθηγητης,θελω να εχω δυνατοτητα να βαζω βαθμολογια στους μαθητες που παρακολουθουν το μαθημα/μαθηματα που διδασκω.</t>
   </si>
   <si>
-    <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Δηλωση Βαθμολογιας" το οποιο θα οδηγει τον καθηγητη στη φορμα δηλωσης βαθμολογιας φοιτητων.</t>
+    <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Δηλωση Βαθμολογιας" η οποια θα οδηγει τον καθηγητη στο περιβαλλον δηλωσης βαθμολογιας φοιτητων.</t>
   </si>
   <si>
     <t xml:space="preserve">US05</t>
@@ -255,7 +216,7 @@
     <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να προσθετω και να αφαιρω καθηγητη/-ες απο το συστημα.</t>
   </si>
   <si>
-    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Προσθηκη/Αφαιρεση Καθηγητη" το οποιο θα τον οδηγει στο περιβαλλον διαχειρισης καθηγητων.</t>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Προσθηκη/Αφαιρεση Καθηγητη" η οποια θα τον οδηγει στο περιβαλλον διαχειρισης καθηγητων.</t>
   </si>
   <si>
     <t xml:space="preserve">US06</t>
@@ -265,6 +226,105 @@
   </si>
   <si>
     <t xml:space="preserve">Πατώντας την επιλογή  Δήλωση στο συστημα,θα μπορέι ο ταυτοποιήμενος χρήστης να δει τα μαθήματα που δήλωσε.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να προσθετω/αφαιρω μαθημα.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Επεξεργασιας Μαθηματων” η οποια θα οδηγει τον διαχειριστη στο περιβαλλον διαχειρησης μαθηματων.Εκει θα υπαρχει,εκτος αλλων, κουμπι “Προσθηκη Μαθηματος” το οποιο θα τον οδηγησει στην φορμα για την προσθηκη του μαθηματος.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να δηλωνω ημερομηνια και ωρα δηλωσης μαθηματων.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Ορισμος Δηλωσης Μαθηματων” η οποια τον οδηγει στην φορμα οπου,εκτος αλλων,θα υπαρχει πεδιο “Ημερομηνια Εναρξης Δηλωσης Μαθηματων”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να δηλωνω τις ομαδες στις οποιες θα χωριζονται οι φοιτητες και τις ωρες για καθε ομαδα στις οποιες οι φοιτητες που ανηκουν στην ομαδα θα πρεπει να δηλωσουν τα μαθημα.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Ορισμος Δηλωσης Μαθηματων” η οποια θα τον οδηγει στην φορμα οπου,εκτος αλλων,θα υπαρχει κουμπι “Προσθηκη Ομαδας”με το οποιο δηλωνη την ομαδα με βαση καποια κριτιρια.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως διαχειριστης,θελω μετα την προσθηκη των ομαδων για τη δηλωση μαθηματων να βλεπω τον αριθμο των φοιτητων που ανηκουν σε καθε ομαδα.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης ολοκληρωση την προσθηκη της ομαδας,θα του εμφανιζεται ο αριθμος των φοιτητων που ανηκουν στην ομαδα.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να δημιουργω χ αριθμο κωδικων για χ φοιττηες.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Φοιτητες” η οποια θα τον οδηγει στο περιβαλλον διαχειρησης φοιτητων.Εκει,εκτος αλλων,θα υπαρχει κουμπι “Δημιουργια Κωδικων Φοιτητων” το οποιο θα οδηγει τον διαχειριστη στη φορμα οπου θα δηλωνει,εκτος αλλων,εναν αριθμο – τον αριθμο των κωδικων που θελει να δημιουργησει και το κουμπι “Δημιουργια” το οποιο θα δημιουργει και αποθηκευει ολους τους κωδικους</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως φοιτητης,θελω να εχω δυνατοτητα να αλλαζω τον κωδικο μου.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο φοιτητης θα μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Ο λογαριασμος μου” η οποια θα τον οδηγει στην φορμα οπου θα μπορει,εκτος αλλων,να αλλαζει τον κωδικο του.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως φοιτητης,θελω να εχω δυνατοτητα να βλεπω την τρεχουσα βαθμολογια μου στα μαθηματα.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο φοιτητης θα μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Η βαθμολογια μου” η οποια θα οδηγει τον φοιτητη στη λιστα των μαθηματων που δηλωσε και θα εμφανιζει τις αντιστοιχες βαθμολογιες αυτων.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως διαχειριστης,θελω(μετα τη δηλωση μαθηματος με εργαστηριο) να εχω δυνατοτητα προσθεσης/αφαιρεσης εργαστηριων.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Επεξεργασιας Εργαστηριων” οπου,εκτος αλλων,θα υπαρχει δυνατοτητα προσθηκης/αφαιρεσης εργαστηριων.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως καθηγητης που διδασκω καποιο εργαστηριο,θελω να εχω δυνατοτητα να προσθετω φοιτητες στο εργαστηριο.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Τα εργαστηρια μου” οπου,διαλεγωντας το εργαστηριο,θα του ανοιγει φορμα οπου,εκτος αλλων,θα υπαρχει δυνατοτηα προσθηκη φοιτητη.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως καθηγητης που διδασκω καποιο εργαστηριο,θελω να εχω δυνατοτητα να προσθετω απουσιες στους φοιτιτες που παρακολουθουν το εργαστηριο</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο καθηγητης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη “Τα εργαστηρια μου” οπου,διαλεγωντας το εργαστηριο,θα του ανοιγει φορμα οπου,εκτος αλλων,θα υπαρχει λιστα φοιτητων και κουμπι “Αυξηση απουσιων” διπλα σε καθε φοιτητη.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ως φοιτητης,θελω να εχω δυνατοτητα να δηλωνω μαθηματα κατα την δηλωσω των μαθηματων.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο φοιτητης θα μπαινει στο συστημα και εφοσον θα ανηκει στην καταλληλη ομαδα,θα υπαρχει επιλογη “Δηλωση Μαθηματων” η οποια θα τον οδηγει στο περιβαλλον δηλωσης μαθηματων οπου θα μπορει να επιλεγει τα μαθηματα και εργαστηρια τα οποια θελει να παρακολουθηση.</t>
   </si>
 </sst>
 </file>
@@ -275,7 +335,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -287,19 +347,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="161"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="161"/>
     </font>
     <font>
       <b val="true"/>
@@ -392,6 +449,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -442,7 +505,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -535,11 +598,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,14 +697,11 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,20 +928,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -959,7 +1026,7 @@
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="89.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
         <v>49</v>
       </c>
@@ -972,7 +1039,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" customFormat="false" ht="89.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
         <v>52</v>
       </c>
@@ -985,7 +1052,7 @@
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" customFormat="false" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="65.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
         <v>55</v>
       </c>
@@ -998,148 +1065,202 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+    <row r="11" customFormat="false" ht="56.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" customFormat="false" ht="45.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+    <row r="12" customFormat="false" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>63</v>
+      </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+    <row r="13" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+    <row r="14" customFormat="false" ht="86.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" customFormat="false" ht="42.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>72</v>
+      </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+    <row r="16" customFormat="false" ht="46.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>75</v>
+      </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+    <row r="17" customFormat="false" ht="50.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>78</v>
+      </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
+    <row r="18" customFormat="false" ht="40.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+    <row r="20" customFormat="false" ht="57.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>87</v>
+      </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-    </row>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added 7 user stories to the main User_Stories file.
</commit_message>
<xml_diff>
--- a/UserStories/arslan/User_Stories.xlsx
+++ b/UserStories/arslan/User_Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Διεργασία" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="274">
   <si>
     <t xml:space="preserve"> Βήματα διεργασίας SCRUM</t>
   </si>
@@ -150,7 +150,7 @@
     <t xml:space="preserve">Ως logout χρηστης θέλω να κάνω login για να εχω προσβαση στο συστημα.</t>
   </si>
   <si>
-    <t xml:space="preserve">Στο UI εισάγω τα διαπιστευτήριά μου (username, passw) με τα οποία, μετά τον έλεγχο, εισάγομαι στην εφαρμογή</t>
+    <t xml:space="preserve">Στο UI εισάγω τα διαπιστευτήριά μου (αριθμος μητρωου, κωδικος) με τα οποία, μετά τον έλεγχο, εισάγομαι στην εφαρμογή</t>
   </si>
   <si>
     <t xml:space="preserve">US03</t>
@@ -179,7 +179,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Πατώντας "Logout" εξέρχομαι από την εφαρμογή και ενημερώνεται ο λογαριασμός μου</t>
+    <t xml:space="preserve">Πατώντας "Logout",εξέρχομαι από την εφαρμογή.</t>
   </si>
   <si>
     <t xml:space="preserve">US04</t>
@@ -765,7 +765,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα φωρτωνει την λιστα ολων των φοιτητων που παρακολουθουν το μαθημα που επελεξα σε μορφη </t>
+      <t xml:space="preserve">το συστημα φορτωνει την λιστα ολων των φοιτητων που παρακολουθουν το μαθημα που επελεξα σε μορφη </t>
     </r>
     <r>
       <rPr>
@@ -924,6 +924,30 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">Τότε </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">το συστημα μου ανοιγει φορμα δηλωσης βαθμολογιας η οποια περιεχει μια λιστα της μορφης [Ονομα Μαθηματος][Τυπος(Εργ. Ή Θεω.)].</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Τοτε </t>
     </r>
     <r>
@@ -1078,7 +1102,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">πατησω το κουμπι Αλλαγη,</t>
+      <t xml:space="preserve">πατησω το κουμπι Καταχωρηση,</t>
     </r>
   </si>
   <si>
@@ -1102,7 +1126,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα εμφανιζει μηνυμα της μορφης [ΑΜ][Ονομα Φοιτητη][Καινουριους βαθμοθς =][Καινουριος Βαθμος]</t>
+      <t xml:space="preserve">το συστημα εμφανιζει μηνυμα της μορφης [ΑΜ][Ονομα Φοιτητη][Καινουριους βαθμος =][Καινουριος Βαθμος]</t>
     </r>
   </si>
   <si>
@@ -2499,7 +2523,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">γεμισω τα πεδια Νεος Κωδικος και Επαναληψη Κωδικου με το νεο μου κωδικο,</t>
+      <t xml:space="preserve">γεμισω τα πεδια Νεος Κωδικος και Επαναληψη Κωδικου με το νεο μου κωδικο</t>
     </r>
   </si>
   <si>
@@ -2645,7 +2669,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">το συστημα μου εμφανιζει ολα τα μαθηματα του ΠΣ και διπλα τη βαθμολογια τους</t>
+      <t xml:space="preserve">το συστημα μου εμφανιζει ολα τα μαθηματα του ΠΣ και διπλα τη βαθμολογια που εχω για καθε μαθημα.</t>
     </r>
   </si>
   <si>
@@ -4493,7 +4517,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4600,12 +4624,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -4746,7 +4764,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4831,8 +4849,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -4840,10 +4858,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4859,27 +4873,27 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4966,7 +4980,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
@@ -5199,8 +5213,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5481,7 +5495,7 @@
       <c r="B25" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="19" t="s">
         <v>102</v>
       </c>
     </row>
@@ -5531,1222 +5545,1222 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D225" activeCellId="0" sqref="D225"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A196" activeCellId="0" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="69.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="22" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="69.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="21" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="24"/>
+      <c r="B3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="29" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31"/>
-      <c r="B19" s="30" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="29" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31"/>
-      <c r="B26" s="30" t="s">
+      <c r="A26" s="30"/>
+      <c r="B26" s="29" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31"/>
-      <c r="B27" s="30" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="29" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31"/>
-      <c r="B28" s="30" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="29" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31"/>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="30"/>
+      <c r="B29" s="29" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="28" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="29" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="29" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31"/>
-      <c r="B38" s="30" t="s">
-        <v>121</v>
+      <c r="A38" s="30"/>
+      <c r="B38" s="29" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31"/>
-      <c r="B39" s="30" t="s">
+      <c r="A39" s="30"/>
+      <c r="B39" s="29" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31"/>
-      <c r="B40" s="30" t="s">
-        <v>128</v>
+      <c r="A40" s="30"/>
+      <c r="B40" s="29" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="31" t="s">
-        <v>129</v>
+      <c r="B41" s="30" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="31" t="s">
-        <v>130</v>
+      <c r="B42" s="30" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="31" t="s">
-        <v>131</v>
+      <c r="B43" s="30" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="31" t="s">
-        <v>132</v>
+      <c r="B44" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="31" t="s">
-        <v>133</v>
+      <c r="B45" s="30" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="31" t="s">
-        <v>134</v>
+      <c r="B46" s="30" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="31" t="s">
-        <v>135</v>
+      <c r="B47" s="30" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="27" t="s">
-        <v>136</v>
+      <c r="B49" s="26" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="29" t="s">
-        <v>137</v>
+      <c r="B51" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="30" t="s">
-        <v>138</v>
+      <c r="B52" s="29" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="30"/>
+      <c r="B54" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31"/>
-      <c r="B54" s="30" t="s">
+    <row r="61" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="29" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="30" t="s">
+    <row r="62" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="30"/>
+      <c r="B72" s="30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="30"/>
+      <c r="B73" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="29" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B67" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="28" t="s">
+    <row r="89" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="29" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="30"/>
+      <c r="B90" s="29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B97" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="29" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="31"/>
-      <c r="B72" s="31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="31"/>
-      <c r="B73" s="30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="31" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="31" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="B85" s="27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="28" t="s">
+    <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="29" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="30"/>
+      <c r="B102" s="30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="30"/>
+      <c r="B103" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B107" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="31"/>
-      <c r="B90" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="31" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B97" s="33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="28" t="s">
+    <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="30"/>
+      <c r="B112" s="29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B117" s="32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="30" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="31"/>
-      <c r="B102" s="31" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="31"/>
-      <c r="B103" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B107" s="33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="28" t="s">
+    <row r="119" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="30"/>
+      <c r="B122" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="30" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="31"/>
-      <c r="B112" s="30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="31" t="s">
+    <row r="126" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="28" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="30"/>
+      <c r="B129" s="29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B144" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="30"/>
+      <c r="B149" s="29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B157" s="32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="30"/>
+      <c r="B162" s="29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B163" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="30" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B170" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B171" s="29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B172" s="29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B175" s="30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B176" s="30" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B177" s="30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B178" s="30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B180" s="32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B181" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B182" s="28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B184" s="30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B185" s="30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B186" s="30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B187" s="30" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B188" s="30" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B189" s="30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B190" s="30" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B191" s="30" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B192" s="30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B193" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B194" s="30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B196" s="32" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B197" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B198" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B199" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B200" s="30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="132.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B201" s="30" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B202" s="30" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B203" s="30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B204" s="30" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B205" s="30" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B117" s="33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="28" t="s">
+    <row r="206" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B206" s="30" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B207" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B208" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B210" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B211" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="30" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="30" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="31"/>
-      <c r="B122" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B124" s="33" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="28" t="s">
+    <row r="212" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B212" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B213" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B214" s="30" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B215" s="30" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B216" s="30" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B217" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B218" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B220" s="32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B221" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="29" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="31"/>
-      <c r="B129" s="30" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="31" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="31" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="31" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="31" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="29" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="31" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="31" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B144" s="33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="28" t="s">
+    <row r="222" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B222" s="28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B223" s="30" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B224" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B225" s="30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B226" s="30" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B227" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B228" s="30" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B229" s="30" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B230" s="30" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B232" s="32" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B233" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="31"/>
-      <c r="B149" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="31" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="31" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B157" s="33" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="29" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="31"/>
-      <c r="B162" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="31" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="31" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="31" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B168" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="31" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="31" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="31" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="31" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B180" s="33" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B181" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="29" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B183" s="30" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B184" s="31" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B185" s="31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B186" s="31" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B187" s="31" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B188" s="31" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B189" s="31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B190" s="31" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B191" s="31" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B192" s="31" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B193" s="31" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B196" s="33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B197" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="29" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B199" s="31" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="132.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B201" s="31" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B202" s="31" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B203" s="31" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="31" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B205" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B206" s="31" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B207" s="31" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B208" s="31" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B210" s="33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="31" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="31" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B215" s="31" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B216" s="31" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B217" s="31" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B218" s="31" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="B220" s="33" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B221" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="31" t="s">
+    <row r="234" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B234" s="28" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B224" s="31" t="s">
+    <row r="235" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B235" s="30" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="31" t="s">
+    <row r="236" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B236" s="30" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B226" s="31" t="s">
+    <row r="237" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B237" s="30" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B227" s="31" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B228" s="31" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B229" s="31" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B230" s="31" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="B232" s="33" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B234" s="29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B235" s="31" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="236" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B236" s="31" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B237" s="31" t="s">
-        <v>261</v>
-      </c>
-    </row>
     <row r="238" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="31" t="s">
-        <v>268</v>
+      <c r="B238" s="30" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B239" s="31" t="s">
-        <v>269</v>
+      <c r="B239" s="30" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B240" s="31" t="s">
-        <v>270</v>
+      <c r="B240" s="30" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B241" s="31" t="s">
-        <v>271</v>
+      <c r="B241" s="30" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B242" s="31" t="s">
-        <v>272</v>
+      <c r="B242" s="30" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Changes: 1)Made sequence diagramms for user stories 2,5,6,9,10,11.
</commit_message>
<xml_diff>
--- a/UserStories/arslan/User_Stories.xlsx
+++ b/UserStories/arslan/User_Stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Διεργασία" sheetId="1" state="visible" r:id="rId2"/>
@@ -4980,7 +4980,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
@@ -5213,8 +5213,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5356,7 +5356,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="61.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
         <v>64</v>
       </c>
@@ -5545,8 +5545,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A196" activeCellId="0" sqref="A196"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A176" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B176" activeCellId="0" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Allages: 1)Prosthesa 2 kainouria user stories(diagrammata akolouthias,kritiria apodoxhs) 2)Allages to enoiologiko montelo kai prosthesa kainourious methodous apo ta kainouria user stories.
</commit_message>
<xml_diff>
--- a/UserStories/arslan/User_Stories.xlsx
+++ b/UserStories/arslan/User_Stories.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="269">
   <si>
     <t xml:space="preserve"> Βήματα διεργασίας SCRUM</t>
   </si>
@@ -212,10 +212,10 @@
     <t xml:space="preserve">US07</t>
   </si>
   <si>
-    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να προσθετω/αφαιρω μαθημα στο ΠΣ για να μπορω να δηλωνω καινουρια μαθηματα και να αφαιρω μη-διδακταια μαθηματα.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Επεξεργασιας Μαθηματων” η οποια θα οδηγει τον διαχειριστη στο περιβαλλον διαχειρησης μαθηματων.</t>
+    <t xml:space="preserve">Ως διαχειριστης,θελω να εχω δυνατοτητα να προσθετω μαθημα στο ΠΣ για να μπορω να δηλωνω καινουρια μαθηματα.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Οταν ο διαχειριστης μπαινει στο συστημα,θα υπαρχει στο μενου επιλογη "Επεξεργασιας Μαθηματων” η οποια θα οδηγει τον διαχειριστη στο περιβαλλον διαχειρησης μαθηματων.Οπου,συμπληρωνοντας ολα τα πεδια,θα υπαρχει κουμπι προσθηκη για προσθηκη μαθηματος στο ΠΣ(ειτε εργαστηριο ειτε θεωρια)</t>
   </si>
   <si>
     <t xml:space="preserve">US08</t>
@@ -1620,7 +1620,7 @@
         <family val="2"/>
         <charset val="161"/>
       </rPr>
-      <t xml:space="preserve">Αφαιρεση υπαρχοντος μαθηματος</t>
+      <t xml:space="preserve">Προσθηκη καινουριου μαθηματος</t>
     </r>
   </si>
   <si>
@@ -1720,199 +1720,6 @@
     <r>
       <rPr>
         <b val="true"/>
-        <i val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Οταν </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">πατησω το κουμπι Διαγραφη διπλα σε καποιο μαθηματα,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τοτε</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> το συστημα εμφανιζει μηνυμα της μορφης </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Θελετε να διαγραψετε το μαθημα][Ονομα Μαθηματος]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> και δυο κουμπια </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Ναι]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> και </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Οχι]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Και οταν</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> πατησω το κουμπι [Ναι] για επιβεβαιωση,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Τοτε</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> το συστημα εμφανιζει μηνυμα της μορφης </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[Ονομα Μαθηματος]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> αφαιρεθηκε επιτυχως</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="16"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-      </rPr>
-      <t xml:space="preserve">Σενάριο: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-      </rPr>
-      <t xml:space="preserve">Προσθηκη καινουριου μαθηματος</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
         <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
@@ -1929,7 +1736,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> γεμισω την φορμα – ονομα μαθηματος,εξαμηνο,αν εχει εργαστηριακο μερος,κωδικος μαθηματος,Ονομα καθηγητη που διδασκει την θεωρια,αν ειναι μαθημα κατευθυνσης</t>
+      <t xml:space="preserve"> γεμισω την φορμα – ονομα μαθηματος,εξαμηνο,αν εχει εργαστηριακο μερος(αν ειναι μαθημα θεωριας),Ονομα καθηγητη που διδασκει την θεωρια/εργαστηριο,τα προαπαιτοθμενα μαθηματα θεωριας(αν ειναι θεωρια)</t>
     </r>
   </si>
   <si>
@@ -4980,7 +4787,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.41"/>
@@ -5213,8 +5020,8 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5323,7 +5130,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="54.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="82.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>55</v>
       </c>
@@ -5545,8 +5352,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A176" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B176" activeCellId="0" sqref="B176"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5894,7 +5701,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="25" t="s">
         <v>55</v>
       </c>
@@ -5923,241 +5730,238 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="30"/>
       <c r="B72" s="30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="30"/>
-      <c r="B73" s="29" t="s">
+    <row r="73" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="22" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="30" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="30" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="30" t="s">
+    <row r="77" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="25" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="28" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="22" t="s">
+    <row r="80" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="29" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="30" t="s">
+    <row r="82" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="30"/>
+      <c r="B82" s="29" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="30" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="25" t="s">
+    <row r="84" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="B85" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="27" t="s">
+    </row>
+    <row r="85" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B89" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="29" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="30"/>
-      <c r="B90" s="29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="30" t="s">
+    <row r="91" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="28" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="30" t="s">
+    <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="29" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="30" t="s">
+    <row r="93" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="29" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="30"/>
       <c r="B94" s="30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="30" t="s">
+    <row r="95" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="30"/>
+      <c r="B95" s="29" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B97" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="27" t="s">
+    <row r="96" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="28" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="29" t="s">
-        <v>173</v>
-      </c>
-    </row>
     <row r="101" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="30"/>
-      <c r="B102" s="30" t="s">
+    <row r="102" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="29" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="30"/>
+    <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="29" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="30" t="s">
+    <row r="104" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="30"/>
+      <c r="B104" s="29" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B107" s="32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="27" t="s">
+    <row r="106" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="28" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="29" t="s">
-        <v>180</v>
-      </c>
-    </row>
     <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="30"/>
+      <c r="B111" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="30" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="30" t="s">
+    <row r="113" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="29" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="30" t="s">
+    <row r="114" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="30"/>
+      <c r="B114" s="29" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B117" s="32" t="s">
+    <row r="116" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B116" s="32" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="27" t="s">
+    <row r="117" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="28" t="s">
+    <row r="118" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="28" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="29" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6165,604 +5969,573 @@
         <v>188</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="30"/>
       <c r="B121" s="29" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="30"/>
-      <c r="B122" s="29" t="s">
+    <row r="122" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="30" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B124" s="32" t="s">
+    <row r="123" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="30" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="28" t="s">
+    <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="30" t="s">
         <v>192</v>
       </c>
     </row>
+    <row r="125" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
     <row r="127" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="29" t="s">
-        <v>139</v>
+      <c r="B127" s="28" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="30"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="30" t="s">
-        <v>195</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="29" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="30" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="30" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="30" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="28" t="s">
+    <row r="136" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="28" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="29" t="s">
+    <row r="139" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="29" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="30" t="s">
+    <row r="140" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="29" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="30" t="s">
+    <row r="141" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="30"/>
+      <c r="B141" s="29" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="30" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="30" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B144" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="27" t="s">
+    <row r="143" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B149" s="32" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="28" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="30"/>
-      <c r="B149" s="29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="30" t="s">
+    <row r="151" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="28" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="30" t="s">
+    <row r="152" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="30"/>
+      <c r="B154" s="29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="30" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="30" t="s">
+    <row r="157" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="30" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="30" t="s">
+    <row r="158" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="30" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="B157" s="32" t="s">
+    <row r="159" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="30" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="28" t="s">
+    <row r="160" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="30" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="29" t="s">
-        <v>206</v>
-      </c>
-    </row>
     <row r="161" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="30"/>
+      <c r="B161" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B163" s="29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="30" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="30" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B170" s="30" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="28" t="s">
+    <row r="172" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B172" s="32" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="30" t="s">
+    <row r="173" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="28" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="30" t="s">
+    <row r="175" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B175" s="29" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="30" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="30" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B180" s="32" t="s">
+    <row r="179" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B179" s="30" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B181" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="28" t="s">
+    <row r="180" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B180" s="30" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B183" s="29" t="s">
+    <row r="181" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B181" s="30" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B182" s="30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="30" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="30" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="30" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="30" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B187" s="30" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B188" s="30" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B189" s="30" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B190" s="30" t="s">
+    <row r="188" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B188" s="32" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B189" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B190" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="30" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="132.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B193" s="30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B194" s="30" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B195" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B196" s="30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B197" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B198" s="30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B199" s="30" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B200" s="30" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B202" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B203" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B204" s="28" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B205" s="30" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B193" s="30" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="30" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B196" s="32" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B197" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="28" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B199" s="30" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="30" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="132.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B201" s="30" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B202" s="30" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B203" s="30" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="30" t="s">
+    <row r="206" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B206" s="30" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B205" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B206" s="30" t="s">
+    <row r="207" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B207" s="30" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B207" s="30" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B209" s="30" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B210" s="32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="27" t="s">
+    <row r="210" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B210" s="30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B212" s="32" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B213" s="27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="30" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="30" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="94.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B214" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="30" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B217" s="30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B218" s="30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B219" s="30" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B220" s="30" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B221" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B222" s="30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B224" s="32" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B225" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B226" s="28" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B217" s="30" t="s">
+    <row r="227" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B227" s="30" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B218" s="30" t="s">
+    <row r="228" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B228" s="30" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="25" t="s">
+    <row r="229" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B229" s="30" t="s">
         <v>257</v>
-      </c>
-      <c r="B220" s="32" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B221" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="30" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B224" s="30" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="30" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="226" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B226" s="30" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B227" s="30" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B228" s="30" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B229" s="30" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B231" s="30" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B232" s="30" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B233" s="30" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B232" s="32" t="s">
+    <row r="234" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B234" s="30" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B234" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B235" s="30" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="236" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B236" s="30" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B237" s="30" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="30" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B239" s="30" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B240" s="30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B241" s="30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B242" s="30" t="s">
-        <v>273</v>
-      </c>
-    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>